<commit_message>
Added training files for testing
</commit_message>
<xml_diff>
--- a/Training/Section_Master.xlsx
+++ b/Training/Section_Master.xlsx
@@ -1,49 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\FMSResources\Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E09D89E-8F03-40BC-83BE-A5412C27CD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D4C56-7937-4B54-8786-25648EA4A2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Section Master" sheetId="8" r:id="rId1"/>
+    <sheet name="General" sheetId="5" r:id="rId2"/>
+    <sheet name="NCI, JV, Associates" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t>Topic Name</t>
+  </si>
+  <si>
+    <t>Topic File Name</t>
+  </si>
+  <si>
+    <t>Report Validation</t>
+  </si>
+  <si>
+    <t>Report_Validation.xlsx</t>
+  </si>
+  <si>
+    <t>User Role Management</t>
+  </si>
+  <si>
+    <t>User_Role_Management.xlsx</t>
+  </si>
+  <si>
+    <t>Taxonomy config for NCI</t>
+  </si>
+  <si>
+    <t>Taxonomy_config.xlsx</t>
+  </si>
+  <si>
+    <t>Auto journal setup for NCI</t>
+  </si>
+  <si>
+    <t>Auto_journal_setup.xlsx</t>
+  </si>
+  <si>
+    <t>Sec Order</t>
+  </si>
+  <si>
+    <t>Section Name</t>
+  </si>
+  <si>
+    <t>Section Key</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
   <si>
     <t>Topic Key</t>
   </si>
   <si>
-    <t>Topic Name</t>
-  </si>
-  <si>
-    <t>Topic File Name</t>
-  </si>
-  <si>
-    <t>FA Schedule</t>
+    <t>NCI, JV, Associates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,13 +109,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,15 +160,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{5D03A933-3196-4534-B158-56FC5185FB9B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,40 +452,849 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230D77F9-0FA0-4697-B7FB-32447BF547D2}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="29.90625" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="str">
+        <f>LOWER(SUBSTITUTE(TRIM(B2)," ","_"))</f>
+        <v>general</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="str">
+        <f>LOWER(SUBSTITUTE(TRIM(B3)," ","_"))</f>
+        <v>nci,_jv,_associates</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C31" si="0">LOWER(SUBSTITUTE(TRIM(B4)," ","_"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D41063-3216-434C-A1CE-94FDD1117DB4}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" customWidth="1"/>
+    <col min="5" max="5" width="31.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" t="str">
+        <f>LOWER(SUBSTITUTE(TRIM(B2)," ","_"))</f>
+        <v>report_validation</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D33" si="0">LOWER(SUBSTITUTE(TRIM(B3)," ","_"))</f>
+        <v>user_role_management</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA1A617-A6D5-4FD6-96D4-E56A0D4F1C65}">
+  <dimension ref="A1:D56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="str">
+        <f>LOWER(SUBSTITUTE(TRIM(B2)," ","_"))</f>
+        <v>taxonomy_config_for_nci</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D56" si="0">LOWER(SUBSTITUTE(TRIM(B3)," ","_"))</f>
+        <v>auto_journal_setup_for_nci</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>